<commit_message>
Adding updated cal sheets.
</commit_message>
<xml_diff>
--- a/CP02PMCI/Omaha_Cal_Info_CP02PMCI_00001.xlsx
+++ b/CP02PMCI/Omaha_Cal_Info_CP02PMCI_00001.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="4512" windowWidth="18744" windowHeight="4332" tabRatio="377" activeTab="1"/>
+    <workbookView xWindow="-12" yWindow="5544" windowWidth="23064" windowHeight="5580" tabRatio="377" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -32,12 +32,12 @@
     <definedName name="_FilterDatabase_1_1_1_1_1_1">Moorings!$A$1:$J$102</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$406</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="65">
   <si>
     <t>Ref Des</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>CP02PMCI</t>
-  </si>
-  <si>
     <t>CP02PMCI-00001</t>
   </si>
   <si>
@@ -135,6 +132,9 @@
     <t>CP02PMCI-WFP01-04-FLORTK000</t>
   </si>
   <si>
+    <t>CC_angular resolution</t>
+  </si>
+  <si>
     <t>CC_dark_counts_cdom</t>
   </si>
   <si>
@@ -144,6 +144,12 @@
     <t>CC_dark_counts_volume_scatter</t>
   </si>
   <si>
+    <t>CC_depolarization ratio</t>
+  </si>
+  <si>
+    <t>CC_measurement wavelength</t>
+  </si>
+  <si>
     <t>CC_scale_factor_cdom</t>
   </si>
   <si>
@@ -151,6 +157,9 @@
   </si>
   <si>
     <t>CC_scale_factor_volume_scatter</t>
+  </si>
+  <si>
+    <t>CC_scattering angle</t>
   </si>
   <si>
     <t>CP02PMCI-WFP01-05-PARADK000</t>
@@ -212,22 +221,19 @@
     <t>SWE0008-G</t>
   </si>
   <si>
+    <t>CP02PMCI-PM001</t>
+  </si>
+  <si>
     <t>40°13.612'N</t>
   </si>
   <si>
     <t>70°53.336'W</t>
   </si>
   <si>
-    <t>CC_angular_resolution</t>
-  </si>
-  <si>
-    <t>CC_depolarization_ratio</t>
-  </si>
-  <si>
-    <t>CC_measurement_wavelength</t>
-  </si>
-  <si>
-    <t>CC_scattering_angle</t>
+    <t>CC_dark_offset</t>
+  </si>
+  <si>
+    <t>CC_scale_wet</t>
   </si>
 </sst>
 </file>
@@ -239,7 +245,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -333,6 +339,13 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -724,7 +737,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -787,6 +800,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="289">
     <cellStyle name="Comma 2" xfId="266"/>
@@ -1447,7 +1463,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1473,7 +1489,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -1502,10 +1518,10 @@
     </row>
     <row r="2" spans="1:11" s="21" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="17">
         <v>1</v>
@@ -1520,16 +1536,16 @@
         <v>41948</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K2" s="20"/>
     </row>
@@ -1543,8 +1559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1569,19 +1585,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>16</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>9</v>
@@ -1589,10 +1605,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="5">
         <v>1</v>
@@ -1601,21 +1617,21 @@
         <v>18596</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="4">
         <v>119</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="5">
         <v>1</v>
@@ -1624,7 +1640,7 @@
         <v>18596</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="4">
         <v>40.226866666666666</v>
@@ -1632,10 +1648,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="5">
         <v>1</v>
@@ -1644,7 +1660,7 @@
         <v>18596</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" s="4">
         <v>-70.888933333333298</v>
@@ -1657,16 +1673,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="5">
         <v>1</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1674,15 +1690,15 @@
       <c r="C7" s="5"/>
       <c r="F7" s="12"/>
       <c r="G7" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="5">
         <v>1</v>
@@ -1691,21 +1707,21 @@
         <v>2724</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F8" s="4">
         <v>40.226866666666666</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="5">
         <v>1</v>
@@ -1714,7 +1730,7 @@
         <v>2724</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9" s="4">
         <v>-70.888933333333298</v>
@@ -1722,10 +1738,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="5">
         <v>1</v>
@@ -1734,7 +1750,7 @@
         <v>2724</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10" s="14">
         <v>-791.56</v>
@@ -1742,10 +1758,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="5">
         <v>1</v>
@@ -1754,7 +1770,7 @@
         <v>2724</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F11" s="16">
         <v>2.4876E-4</v>
@@ -1762,10 +1778,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="5">
         <v>1</v>
@@ -1774,7 +1790,7 @@
         <v>2724</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F12" s="16">
         <v>-3.0284999999999999E-3</v>
@@ -1782,10 +1798,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="5">
         <v>1</v>
@@ -1794,7 +1810,7 @@
         <v>2724</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F13" s="16">
         <v>1.6759000000000001E-4</v>
@@ -1802,10 +1818,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="5">
         <v>1</v>
@@ -1814,7 +1830,7 @@
         <v>2724</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F14" s="16">
         <v>-2.3502E-6</v>
@@ -1822,10 +1838,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" s="5">
         <v>1</v>
@@ -1834,7 +1850,7 @@
         <v>2724</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15" s="14">
         <v>3.5999999999999997E-2</v>
@@ -1847,10 +1863,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" s="5">
         <v>1</v>
@@ -1859,21 +1875,21 @@
         <v>125</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F17" s="4">
         <v>40.226866666666666</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" s="5">
         <v>1</v>
@@ -1882,7 +1898,7 @@
         <v>125</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F18" s="4">
         <v>-70.888933333333298</v>
@@ -1895,10 +1911,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" s="5">
         <v>1</v>
@@ -1907,21 +1923,21 @@
         <v>100037</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F20" s="4">
         <v>40.226866666666666</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C21" s="5">
         <v>1</v>
@@ -1930,7 +1946,7 @@
         <v>100037</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F21" s="4">
         <v>-70.888933333333298</v>
@@ -1942,10 +1958,10 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C23" s="5">
         <v>1</v>
@@ -1954,21 +1970,21 @@
         <v>1119</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="F23" s="4">
         <v>1.08</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C24" s="5">
         <v>1</v>
@@ -1977,21 +1993,21 @@
         <v>1119</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="F24" s="4">
         <v>3.9E-2</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C25" s="5">
         <v>1</v>
@@ -2000,7 +2016,7 @@
         <v>1119</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="F25" s="4">
         <v>700</v>
@@ -2008,10 +2024,10 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C26" s="5">
         <v>1</v>
@@ -2020,7 +2036,7 @@
         <v>1119</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="F26" s="4">
         <v>117</v>
@@ -2028,10 +2044,10 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C27" s="5">
         <v>1</v>
@@ -2046,15 +2062,15 @@
         <v>60</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C28" s="5">
         <v>1</v>
@@ -2071,10 +2087,10 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C29" s="5">
         <v>1</v>
@@ -2091,10 +2107,10 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C30" s="5">
         <v>1</v>
@@ -2103,7 +2119,7 @@
         <v>1119</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F30" s="13">
         <v>9.0399999999999994E-2</v>
@@ -2111,10 +2127,10 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C31" s="5">
         <v>1</v>
@@ -2123,7 +2139,7 @@
         <v>1119</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F31" s="13">
         <v>1.2500000000000001E-2</v>
@@ -2131,10 +2147,10 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C32" s="5">
         <v>1</v>
@@ -2143,7 +2159,7 @@
         <v>1119</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F32" s="15">
         <v>3.095E-6</v>
@@ -2156,10 +2172,10 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C34" s="5">
         <v>1</v>
@@ -2167,22 +2183,22 @@
       <c r="D34" s="13">
         <v>20465</v>
       </c>
-      <c r="E34" s="4" t="s">
-        <v>33</v>
+      <c r="E34" s="22" t="s">
+        <v>63</v>
       </c>
       <c r="F34" s="13">
         <v>1</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C35" s="5">
         <v>1</v>
@@ -2190,8 +2206,8 @@
       <c r="D35" s="13">
         <v>20465</v>
       </c>
-      <c r="E35" s="4" t="s">
-        <v>36</v>
+      <c r="E35" s="22" t="s">
+        <v>64</v>
       </c>
       <c r="F35" s="15">
         <v>1.01E-17</v>
@@ -2204,30 +2220,30 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C37" s="5">
         <v>1</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C39" s="5">
         <v>1</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Reverting outdated cal files for CP02PMCI to correct cal files.
</commit_message>
<xml_diff>
--- a/CP02PMCI/Omaha_Cal_Info_CP02PMCI_00001.xlsx
+++ b/CP02PMCI/Omaha_Cal_Info_CP02PMCI_00001.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="5544" windowWidth="23064" windowHeight="5580" tabRatio="377" activeTab="1"/>
+    <workbookView xWindow="24" yWindow="4512" windowWidth="18744" windowHeight="4332" tabRatio="377" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -32,12 +32,12 @@
     <definedName name="_FilterDatabase_1_1_1_1_1_1">Moorings!$A$1:$J$102</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$406</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="63">
   <si>
     <t>Ref Des</t>
   </si>
@@ -69,6 +69,9 @@
     <t>Notes</t>
   </si>
   <si>
+    <t>CP02PMCI</t>
+  </si>
+  <si>
     <t>CP02PMCI-00001</t>
   </si>
   <si>
@@ -132,9 +135,6 @@
     <t>CP02PMCI-WFP01-04-FLORTK000</t>
   </si>
   <si>
-    <t>CC_angular resolution</t>
-  </si>
-  <si>
     <t>CC_dark_counts_cdom</t>
   </si>
   <si>
@@ -144,12 +144,6 @@
     <t>CC_dark_counts_volume_scatter</t>
   </si>
   <si>
-    <t>CC_depolarization ratio</t>
-  </si>
-  <si>
-    <t>CC_measurement wavelength</t>
-  </si>
-  <si>
     <t>CC_scale_factor_cdom</t>
   </si>
   <si>
@@ -157,9 +151,6 @@
   </si>
   <si>
     <t>CC_scale_factor_volume_scatter</t>
-  </si>
-  <si>
-    <t>CC_scattering angle</t>
   </si>
   <si>
     <t>CP02PMCI-WFP01-05-PARADK000</t>
@@ -221,19 +212,22 @@
     <t>SWE0008-G</t>
   </si>
   <si>
-    <t>CP02PMCI-PM001</t>
-  </si>
-  <si>
     <t>40°13.612'N</t>
   </si>
   <si>
     <t>70°53.336'W</t>
   </si>
   <si>
-    <t>CC_dark_offset</t>
-  </si>
-  <si>
-    <t>CC_scale_wet</t>
+    <t>CC_angular_resolution</t>
+  </si>
+  <si>
+    <t>CC_depolarization_ratio</t>
+  </si>
+  <si>
+    <t>CC_measurement_wavelength</t>
+  </si>
+  <si>
+    <t>CC_scattering_angle</t>
   </si>
 </sst>
 </file>
@@ -245,7 +239,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -339,13 +333,6 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -737,7 +724,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -800,9 +787,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="289">
     <cellStyle name="Comma 2" xfId="266"/>
@@ -1463,7 +1447,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1489,7 +1473,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -1518,10 +1502,10 @@
     </row>
     <row r="2" spans="1:11" s="21" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="17">
         <v>1</v>
@@ -1536,16 +1520,16 @@
         <v>41948</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K2" s="20"/>
     </row>
@@ -1559,8 +1543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1585,19 +1569,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>9</v>
@@ -1605,10 +1589,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="5">
         <v>1</v>
@@ -1617,21 +1601,21 @@
         <v>18596</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2" s="4">
         <v>119</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="5">
         <v>1</v>
@@ -1640,7 +1624,7 @@
         <v>18596</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F3" s="4">
         <v>40.226866666666666</v>
@@ -1648,10 +1632,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="5">
         <v>1</v>
@@ -1660,7 +1644,7 @@
         <v>18596</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" s="4">
         <v>-70.888933333333298</v>
@@ -1673,16 +1657,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="5">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1690,15 +1674,15 @@
       <c r="C7" s="5"/>
       <c r="F7" s="12"/>
       <c r="G7" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" s="5">
         <v>1</v>
@@ -1707,21 +1691,21 @@
         <v>2724</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F8" s="4">
         <v>40.226866666666666</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" s="5">
         <v>1</v>
@@ -1730,7 +1714,7 @@
         <v>2724</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F9" s="4">
         <v>-70.888933333333298</v>
@@ -1738,10 +1722,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" s="5">
         <v>1</v>
@@ -1750,7 +1734,7 @@
         <v>2724</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F10" s="14">
         <v>-791.56</v>
@@ -1758,10 +1742,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" s="5">
         <v>1</v>
@@ -1770,7 +1754,7 @@
         <v>2724</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F11" s="16">
         <v>2.4876E-4</v>
@@ -1778,10 +1762,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="5">
         <v>1</v>
@@ -1790,7 +1774,7 @@
         <v>2724</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F12" s="16">
         <v>-3.0284999999999999E-3</v>
@@ -1798,10 +1782,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13" s="5">
         <v>1</v>
@@ -1810,7 +1794,7 @@
         <v>2724</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F13" s="16">
         <v>1.6759000000000001E-4</v>
@@ -1818,10 +1802,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C14" s="5">
         <v>1</v>
@@ -1830,7 +1814,7 @@
         <v>2724</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F14" s="16">
         <v>-2.3502E-6</v>
@@ -1838,10 +1822,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C15" s="5">
         <v>1</v>
@@ -1850,7 +1834,7 @@
         <v>2724</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F15" s="14">
         <v>3.5999999999999997E-2</v>
@@ -1863,10 +1847,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C17" s="5">
         <v>1</v>
@@ -1875,21 +1859,21 @@
         <v>125</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F17" s="4">
         <v>40.226866666666666</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C18" s="5">
         <v>1</v>
@@ -1898,7 +1882,7 @@
         <v>125</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F18" s="4">
         <v>-70.888933333333298</v>
@@ -1911,10 +1895,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C20" s="5">
         <v>1</v>
@@ -1923,21 +1907,21 @@
         <v>100037</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F20" s="4">
         <v>40.226866666666666</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C21" s="5">
         <v>1</v>
@@ -1946,7 +1930,7 @@
         <v>100037</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F21" s="4">
         <v>-70.888933333333298</v>
@@ -1958,10 +1942,10 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C23" s="5">
         <v>1</v>
@@ -1970,21 +1954,21 @@
         <v>1119</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="F23" s="4">
         <v>1.08</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C24" s="5">
         <v>1</v>
@@ -1993,21 +1977,21 @@
         <v>1119</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="F24" s="4">
         <v>3.9E-2</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C25" s="5">
         <v>1</v>
@@ -2016,7 +2000,7 @@
         <v>1119</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="F25" s="4">
         <v>700</v>
@@ -2024,10 +2008,10 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C26" s="5">
         <v>1</v>
@@ -2036,7 +2020,7 @@
         <v>1119</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="F26" s="4">
         <v>117</v>
@@ -2044,10 +2028,10 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C27" s="5">
         <v>1</v>
@@ -2062,15 +2046,15 @@
         <v>60</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C28" s="5">
         <v>1</v>
@@ -2087,10 +2071,10 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C29" s="5">
         <v>1</v>
@@ -2107,10 +2091,10 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C30" s="5">
         <v>1</v>
@@ -2119,7 +2103,7 @@
         <v>1119</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F30" s="13">
         <v>9.0399999999999994E-2</v>
@@ -2127,10 +2111,10 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C31" s="5">
         <v>1</v>
@@ -2139,7 +2123,7 @@
         <v>1119</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F31" s="13">
         <v>1.2500000000000001E-2</v>
@@ -2147,10 +2131,10 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C32" s="5">
         <v>1</v>
@@ -2159,7 +2143,7 @@
         <v>1119</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F32" s="15">
         <v>3.095E-6</v>
@@ -2172,10 +2156,10 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C34" s="5">
         <v>1</v>
@@ -2183,22 +2167,22 @@
       <c r="D34" s="13">
         <v>20465</v>
       </c>
-      <c r="E34" s="22" t="s">
-        <v>63</v>
+      <c r="E34" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="F34" s="13">
         <v>1</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C35" s="5">
         <v>1</v>
@@ -2206,8 +2190,8 @@
       <c r="D35" s="13">
         <v>20465</v>
       </c>
-      <c r="E35" s="22" t="s">
-        <v>64</v>
+      <c r="E35" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="F35" s="15">
         <v>1.01E-17</v>
@@ -2220,30 +2204,30 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C37" s="5">
         <v>1</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C39" s="5">
         <v>1</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
cp02pmci, cp02pmui, cp05moas gl336, GP02HYPM, GP03FLMA
Changes to cal sheets to

1. remove m from depth
2.  change glider cal file column names from glider to mooring
</commit_message>
<xml_diff>
--- a/CP02PMCI/Omaha_Cal_Info_CP02PMCI_00001.xlsx
+++ b/CP02PMCI/Omaha_Cal_Info_CP02PMCI_00001.xlsx
@@ -32,12 +32,12 @@
     <definedName name="_FilterDatabase_1_1_1_1_1_1">Moorings!$A$1:$J$102</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$406</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="62">
   <si>
     <t>Ref Des</t>
   </si>
@@ -160,9 +160,6 @@
   </si>
   <si>
     <t>Deployment Number</t>
-  </si>
-  <si>
-    <t>127 m</t>
   </si>
   <si>
     <t>6223-4220-11364</t>
@@ -1472,7 +1469,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1545,13 +1542,13 @@
         <v>41948</v>
       </c>
       <c r="G2" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>41</v>
+      <c r="I2" s="17">
+        <v>127</v>
       </c>
       <c r="J2" s="17" t="s">
         <v>12</v>
@@ -1622,7 +1619,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>11</v>
@@ -1640,12 +1637,12 @@
         <v>119</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>11</v>
@@ -1665,7 +1662,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>11</v>
@@ -1699,7 +1696,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1707,7 +1704,7 @@
       <c r="C7" s="5"/>
       <c r="F7" s="12"/>
       <c r="G7" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1730,7 +1727,7 @@
         <v>40.226866666666666</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1898,7 +1895,7 @@
         <v>40.226866666666666</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1946,7 +1943,7 @@
         <v>40.226866666666666</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1987,13 +1984,13 @@
         <v>1119</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F23" s="4">
         <v>1.0760000000000001</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -2010,13 +2007,13 @@
         <v>1119</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F24" s="4">
         <v>3.9E-2</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -2033,7 +2030,7 @@
         <v>1119</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F25" s="4">
         <v>700</v>
@@ -2053,7 +2050,7 @@
         <v>1119</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F26" s="4">
         <v>124</v>
@@ -2079,7 +2076,7 @@
         <v>60</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -2207,7 +2204,7 @@
         <v>1</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -2237,7 +2234,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>11</v>
@@ -2246,21 +2243,21 @@
         <v>1</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="5">
+        <v>1</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C39" s="5">
-        <v>1</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>